<commit_message>
Finished Model of Rev 2 of the PCBA
</commit_message>
<xml_diff>
--- a/EmojiPad_BOM_V1.xlsx
+++ b/EmojiPad_BOM_V1.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\503371\Dropbox\Downloads\EmojiPad\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17484" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$J$35</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
   <si>
     <t xml:space="preserve">Number of Devices: </t>
   </si>
@@ -287,6 +282,75 @@
   </si>
   <si>
     <t>Bill Of Materials -EmojiPad</t>
+  </si>
+  <si>
+    <t>BOTTOM</t>
+  </si>
+  <si>
+    <t>Case Bottom</t>
+  </si>
+  <si>
+    <t>SCREW1-SCREW8</t>
+  </si>
+  <si>
+    <t>Screws for PCB and Case</t>
+  </si>
+  <si>
+    <t>NUT1-NUT4</t>
+  </si>
+  <si>
+    <t>Acorn Nut</t>
+  </si>
+  <si>
+    <t>M3 Size, 10 mm Long, 0.5 mm Pitch, Low Profile Socket Head</t>
+  </si>
+  <si>
+    <t>McMaster-Carr</t>
+  </si>
+  <si>
+    <t>90666A105</t>
+  </si>
+  <si>
+    <t>Aluminum UnThreaded Spacer 4.5 mm OD, 2mm Length</t>
+  </si>
+  <si>
+    <t>94669A210</t>
+  </si>
+  <si>
+    <t>Regular M3 Nut</t>
+  </si>
+  <si>
+    <t>Zinc Plated, M3x0.5 Thread Size, 5.5mm Wide, 1.8mm High</t>
+  </si>
+  <si>
+    <t>90695A033</t>
+  </si>
+  <si>
+    <t>SPACER1-SPACER4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spacer for PCB </t>
+  </si>
+  <si>
+    <t>Acorn Nut M3 Size, .5mm Pitch, 5.5mm Width, 6mm Height</t>
+  </si>
+  <si>
+    <t>94000A330</t>
+  </si>
+  <si>
+    <t>NUT5- NUT8</t>
+  </si>
+  <si>
+    <t>STAND1-STAND5</t>
+  </si>
+  <si>
+    <t>Standoffs</t>
+  </si>
+  <si>
+    <t>98952A218</t>
+  </si>
+  <si>
+    <t>Male-Female Hex Threaded Standoff 4.5mm Hex, 16mm Length</t>
   </si>
 </sst>
 </file>
@@ -296,7 +360,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -384,6 +448,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -408,7 +489,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -441,8 +522,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -463,8 +554,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="42">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -481,6 +575,11 @@
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -496,6 +595,11 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -835,30 +939,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.69921875" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="25.75">
       <c r="A1" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,7 +970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -902,7 +1006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>1</v>
       </c>
@@ -938,7 +1042,7 @@
         <v>30.45</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>2</v>
       </c>
@@ -974,7 +1078,7 @@
         <v>6.8999999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1010,7 +1114,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1046,7 +1150,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1082,7 +1186,7 @@
         <v>3.3000000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>6</v>
       </c>
@@ -1118,7 +1222,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>7</v>
       </c>
@@ -1154,7 +1258,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1190,7 +1294,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>9</v>
       </c>
@@ -1226,7 +1330,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1262,7 +1366,7 @@
         <v>14.850000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>11</v>
       </c>
@@ -1298,7 +1402,7 @@
         <v>6.08</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>12</v>
       </c>
@@ -1334,7 +1438,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1370,7 +1474,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>14</v>
       </c>
@@ -1406,7 +1510,7 @@
         <v>1.5899999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>15</v>
       </c>
@@ -1442,7 +1546,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>16</v>
       </c>
@@ -1475,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>17</v>
       </c>
@@ -1508,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>18</v>
       </c>
@@ -1541,14 +1645,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>19</v>
       </c>
@@ -1561,25 +1665,15 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>20</v>
       </c>
-      <c r="D26" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E26" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F26" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G26" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>87</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7">
@@ -1587,113 +1681,171 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>21</v>
       </c>
-      <c r="D27" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E27" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F27" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G27" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I27" s="7"/>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="str">
+        <f>'Mechanical Component Prices'!B5</f>
+        <v>M3 Size, 10 mm Long, 0.5 mm Pitch, Low Profile Socket Head</v>
+      </c>
+      <c r="E27" t="str">
+        <f>'Mechanical Component Prices'!C5</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="F27" t="str">
+        <f>'Mechanical Component Prices'!D5</f>
+        <v>90666A105</v>
+      </c>
+      <c r="G27" t="str">
+        <f>'Mechanical Component Prices'!E5</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="H27">
+        <f>'Mechanical Component Prices'!F5</f>
+        <v>8</v>
+      </c>
+      <c r="I27">
+        <f>'Mechanical Component Prices'!G5</f>
+        <v>9.1899999999999996E-2</v>
+      </c>
       <c r="J27" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.73519999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>22</v>
       </c>
-      <c r="D28" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E28" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F28" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G28" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I28" s="7"/>
+      <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" t="str">
+        <f>'Mechanical Component Prices'!B6</f>
+        <v>Aluminum UnThreaded Spacer 4.5 mm OD, 2mm Length</v>
+      </c>
+      <c r="E28" t="str">
+        <f>'Mechanical Component Prices'!C6</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="F28" t="str">
+        <f>'Mechanical Component Prices'!D6</f>
+        <v>94669A210</v>
+      </c>
+      <c r="G28" t="str">
+        <f>'Mechanical Component Prices'!E6</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="H28">
+        <f>'Mechanical Component Prices'!F6</f>
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <f>'Mechanical Component Prices'!G6</f>
+        <v>0.35</v>
+      </c>
       <c r="J28" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>23</v>
       </c>
-      <c r="D29" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E29" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F29" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G29" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I29" s="7"/>
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="str">
+        <f>'Mechanical Component Prices'!B7</f>
+        <v>Zinc Plated, M3x0.5 Thread Size, 5.5mm Wide, 1.8mm High</v>
+      </c>
+      <c r="E29" t="str">
+        <f>'Mechanical Component Prices'!C7</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="F29" t="str">
+        <f>'Mechanical Component Prices'!D7</f>
+        <v>90695A033</v>
+      </c>
+      <c r="G29" t="str">
+        <f>'Mechanical Component Prices'!E7</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="H29">
+        <f>'Mechanical Component Prices'!F7</f>
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <f>'Mechanical Component Prices'!G7</f>
+        <v>3.1E-2</v>
+      </c>
       <c r="J29" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>24</v>
       </c>
-      <c r="D30" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E30" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F30" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G30" t="e">
-        <f>'Mechanical Component Prices'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I30" s="7"/>
+      <c r="B30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="str">
+        <f>'Mechanical Component Prices'!B8</f>
+        <v>Acorn Nut M3 Size, .5mm Pitch, 5.5mm Width, 6mm Height</v>
+      </c>
+      <c r="E30" t="str">
+        <f>'Mechanical Component Prices'!C8</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="F30" t="str">
+        <f>'Mechanical Component Prices'!D8</f>
+        <v>94000A330</v>
+      </c>
+      <c r="G30" t="str">
+        <f>'Mechanical Component Prices'!E8</f>
+        <v>McMaster-Carr</v>
+      </c>
+      <c r="H30">
+        <f>'Mechanical Component Prices'!F8</f>
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <f>'Mechanical Component Prices'!G8</f>
+        <v>0.30399999999999999</v>
+      </c>
       <c r="J30" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1.216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" t="s">
+        <v>106</v>
       </c>
       <c r="D31" t="e">
         <f>'Mechanical Component Prices'!#REF!</f>
@@ -1717,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>26</v>
       </c>
@@ -1743,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>27</v>
       </c>
@@ -1769,25 +1921,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="H34" t="s">
         <v>25</v>
       </c>
       <c r="J34" s="7">
         <f>SUM(J6:J33)/C3</f>
-        <v>30.476999999999993</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+        <v>30.824519999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="H35" t="s">
         <v>9</v>
       </c>
       <c r="J35" s="7">
         <f>SUM(J6:J33)</f>
-        <v>304.76999999999992</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>308.24519999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="H37" t="s">
         <v>26</v>
       </c>
@@ -1796,13 +1948,13 @@
         <v>304.76999999999992</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="H38" t="s">
         <v>27</v>
       </c>
       <c r="J38">
         <f>SUM(J25:J31)</f>
-        <v>0</v>
+        <v>3.4752000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1825,19 +1977,19 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="39.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="25.75">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1852,7 +2004,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1887,7 +2039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1922,7 +2074,7 @@
         <v>1.7052799999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1957,7 +2109,7 @@
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1992,7 +2144,7 @@
         <v>7.2450000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2027,7 +2179,7 @@
         <v>8.1699999999999995E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2062,7 +2214,7 @@
         <v>7.8750000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2097,7 +2249,7 @@
         <v>1.44E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2132,7 +2284,7 @@
         <v>2.75E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2167,7 +2319,7 @@
         <v>9.4149999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2202,7 +2354,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2237,7 +2389,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2272,7 +2424,7 @@
         <v>1.2670000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2307,7 +2459,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2342,7 +2494,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2377,7 +2529,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2412,21 +2564,21 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" s="12"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2435,7 +2587,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2448,25 +2600,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="37.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="25.75">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2481,7 +2633,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2516,107 +2668,194 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1</v>
       </c>
+      <c r="B5" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
       <c r="G5">
-        <v>0</v>
+        <f>9.19/100</f>
+        <v>9.1899999999999996E-2</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <f>9.19/100</f>
+        <v>9.1899999999999996E-2</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <f>9.19/100</f>
+        <v>9.1899999999999996E-2</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <f t="shared" ref="J5:K5" si="0">9.19/100</f>
+        <v>9.1899999999999996E-2</v>
       </c>
       <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>9.1899999999999996E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>3</v>
       </c>
+      <c r="B7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
       <c r="G7">
-        <v>0</v>
+        <f>3.1/100</f>
+        <v>3.1E-2</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <f t="shared" ref="H7:K7" si="1">3.1/100</f>
+        <v>3.1E-2</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>3.1E-2</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>3.1E-2</v>
       </c>
       <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>4</v>
       </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
       <c r="G8">
-        <v>0</v>
+        <f>3.04/10</f>
+        <v>0.30399999999999999</v>
       </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <f>3.04/10</f>
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="I8" s="16">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="J8" s="16">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.30399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>5</v>
       </c>
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
       <c r="G9">
-        <v>0</v>
+        <v>1.45</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1.23</v>
       </c>
       <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1.23</v>
+      </c>
+      <c r="J9" s="16">
+        <v>1.23</v>
+      </c>
+      <c r="K9" s="16">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2636,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2656,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2676,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2696,10 +2935,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="24" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:2" ht="24">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="17.5">
       <c r="B21" s="6"/>
     </row>
   </sheetData>

</xml_diff>